<commit_message>
Corrected 2x3 header qty in BOM
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board_BOM.xlsx
+++ b/internal_env_board/internal_env_board_BOM.xlsx
@@ -345,12 +345,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,7 +636,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,15 +648,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -698,11 +698,11 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G10" si="0">F3*E3</f>
-        <v>0.69599999999999995</v>
+        <v>0.34799999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,22 +1045,22 @@
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>6.96</v>
       </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
         <f t="shared" si="1"/>
         <v>6.96</v>
       </c>
@@ -1069,22 +1069,22 @@
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>14.73</v>
       </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
         <f t="shared" si="1"/>
         <v>14.73</v>
       </c>
@@ -1093,22 +1093,22 @@
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.83</v>
       </c>
-      <c r="F20" s="5">
-        <v>1</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
         <f t="shared" si="1"/>
         <v>0.83</v>
       </c>
@@ -1117,22 +1117,22 @@
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>2</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
@@ -1141,22 +1141,22 @@
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0.21</v>
       </c>
-      <c r="F22" s="5">
-        <v>1</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
         <f t="shared" si="1"/>
         <v>0.21</v>
       </c>
@@ -1165,22 +1165,22 @@
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.15</v>
       </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>

</xml_diff>

<commit_message>
Fixed qty 240 ohm res
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board_BOM.xlsx
+++ b/internal_env_board/internal_env_board_BOM.xlsx
@@ -636,7 +636,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,11 +1010,11 @@
         <v>4.7E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>4.7E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed qty JST 2 pin conn
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board_BOM.xlsx
+++ b/internal_env_board/internal_env_board_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -230,9 +230,6 @@
     <t>CON1</t>
   </si>
   <si>
-    <t>CON2-7</t>
-  </si>
-  <si>
     <t>HIH71201</t>
   </si>
   <si>
@@ -279,6 +276,18 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>CON4-7</t>
+  </si>
+  <si>
+    <t>CONN HEADER GH SIDE 2POS 1.25MM</t>
+  </si>
+  <si>
+    <t>SM02B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CON2,3</t>
   </si>
 </sst>
 </file>
@@ -633,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +692,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -707,7 +716,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -731,7 +740,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -755,7 +764,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -779,7 +788,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -827,7 +836,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -851,7 +860,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -899,7 +908,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>30</v>
@@ -923,7 +932,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
@@ -995,7 +1004,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
@@ -1019,7 +1028,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -1043,7 +1052,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>45</v>
@@ -1067,7 +1076,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>48</v>
@@ -1091,7 +1100,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>51</v>
@@ -1163,16 +1172,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E23" s="4">
         <v>0.15</v>
@@ -1183,6 +1192,30 @@
       <c r="G23" s="4">
         <f t="shared" si="1"/>
         <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="4">
+        <f>F24*E24</f>
+        <v>1.84</v>
       </c>
     </row>
   </sheetData>
@@ -1211,8 +1244,9 @@
     <hyperlink ref="D21" r:id="rId19"/>
     <hyperlink ref="D22" r:id="rId20"/>
     <hyperlink ref="D23" r:id="rId21"/>
+    <hyperlink ref="D24" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>